<commit_message>
Refactor README and update application branding to "AirComp能耗计算系统". Enhance user profile management with new update functionality. Introduce energy report generation and storage. Improve sidebar navigation and user interface components. Update API routes and schemas for better organization and clarity.
</commit_message>
<xml_diff>
--- a/backend/app/download/A_空压机概况表.xlsx
+++ b/backend/app/download/A_空压机概况表.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>55</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>27.2</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -482,38 +482,6 @@
         </is>
       </c>
       <c r="F2" t="inlineStr">
-        <is>
-          <t>MH160-2S</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>8.3</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0.7</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
         <is>
           <t>MH55</t>
         </is>
@@ -530,7 +498,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -588,92 +556,45 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MH160-2S</t>
+          <t>MH55</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>64647</t>
+          <t>52453</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>44509</t>
+          <t>28468</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>55</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>(64647-44509)/64647*40%*160=19.9365</t>
+          <t>(52453-28468)/52453*40%*55=10.0599</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>160*(0.3)*7%=3.36</t>
+          <t>55*(0.3)*7%=1.155</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>23.2965</t>
+          <t>11.2149</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t>(160*1.2*0.6885+23.2965)/(27.2*0.6885)=8.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>MH55</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>52453</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>28468</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>(52453-28468)/52453*40%*55=10.0599</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>55*(0.3)*7%=1.155</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>11.2149</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
         <is>
           <t>(55*1.2*0.5427+11.2149)/(8.3*0.5427)=10.44</t>
         </is>
@@ -690,7 +611,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -705,12 +626,6 @@
       <c r="C1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -728,16 +643,6 @@
           <t>英格索兰</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>捷豹</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>英格索兰</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -747,20 +652,10 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ZLS175-2IC</t>
+          <t>ZLS125-2IC</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
-        <is>
-          <t>MH160-2S</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ZLS60-2IC</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
         <is>
           <t>MH55</t>
         </is>
@@ -773,15 +668,9 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>132</v>
+        <v>90</v>
       </c>
       <c r="C4" t="n">
-        <v>160</v>
-      </c>
-      <c r="D4" t="n">
-        <v>45</v>
-      </c>
-      <c r="E4" t="n">
         <v>55</v>
       </c>
     </row>
@@ -792,17 +681,9 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>27.7</v>
+        <v>19.3</v>
       </c>
       <c r="C5" t="inlineStr">
-        <is>
-          <t>27.2</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>9.199999999999999</v>
-      </c>
-      <c r="E5" t="inlineStr">
         <is>
           <t>8.3</t>
         </is>
@@ -824,16 +705,6 @@
           <t>工频</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>变频</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>工频</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -842,15 +713,9 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
       <c r="C7" t="n">
-        <v>8.300000000000001</v>
-      </c>
-      <c r="D7" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="E7" t="n">
         <v>10.44</v>
       </c>
     </row>
@@ -861,15 +726,9 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.095</v>
+        <v>0.09669999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1383</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.1017</v>
-      </c>
-      <c r="E8" t="n">
         <v>0.174</v>
       </c>
     </row>
@@ -880,16 +739,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>31.33</v>
+        <v>44.44</v>
       </c>
       <c r="C9" t="n">
-        <v>31.33</v>
-      </c>
-      <c r="D9" t="n">
-        <v>41.57</v>
-      </c>
-      <c r="E9" t="n">
-        <v>41.57</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="10">
@@ -899,16 +752,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>48.6907</v>
+        <v>20.9004</v>
       </c>
       <c r="C10" t="n">
-        <v>48.6907</v>
-      </c>
-      <c r="D10" t="n">
-        <v>19.5491</v>
-      </c>
-      <c r="E10" t="n">
-        <v>19.5491</v>
+        <v>20.9004</v>
       </c>
     </row>
     <row r="11">
@@ -918,16 +765,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>389526</v>
+        <v>167203</v>
       </c>
       <c r="C11" t="n">
-        <v>389526</v>
-      </c>
-      <c r="D11" t="n">
-        <v>156393</v>
-      </c>
-      <c r="E11" t="n">
-        <v>156393</v>
+        <v>167203</v>
       </c>
     </row>
     <row r="12">
@@ -937,16 +778,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>545919</v>
+        <v>167203</v>
       </c>
       <c r="C12" t="n">
-        <v>545919</v>
-      </c>
-      <c r="D12" t="n">
-        <v>545919</v>
-      </c>
-      <c r="E12" t="n">
-        <v>545919</v>
+        <v>167203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>